<commit_message>
fix: phase 2 - fixbugs: purchasing invoice - cont 2
</commit_message>
<xml_diff>
--- a/exports/transfer_payment_invoice_template.xlsx
+++ b/exports/transfer_payment_invoice_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB6EE52-D53E-AC47-AEBB-E547F6056B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C031C95-F848-F14B-B69A-B3C6F3BFEEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -379,59 +379,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -750,10 +753,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" customHeight="1"/>
@@ -771,36 +774,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:14" ht="17" customHeight="1">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:14" ht="21" customHeight="1">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:14" ht="14" customHeight="1">
       <c r="B4" s="3"/>
@@ -811,62 +814,62 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:14" ht="23" customHeight="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="23"/>
       <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:14" ht="22" customHeight="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="23"/>
       <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:14" ht="20" customHeight="1">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:14" ht="19" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:14" ht="19" customHeight="1">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="14"/>
@@ -874,48 +877,48 @@
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:14" ht="19" customHeight="1">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:14" ht="19" customHeight="1">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="28"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="32"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="18"/>
     </row>
     <row r="12" spans="1:14" ht="21" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="9" t="s">
         <v>11</v>
       </c>
@@ -925,287 +928,191 @@
       <c r="F12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="32"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="18"/>
     </row>
     <row r="13" spans="1:14" ht="23" customHeight="1">
       <c r="A13" s="8"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
     </row>
     <row r="14" spans="1:14" ht="23" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="B14" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-    </row>
-    <row r="15" spans="1:14" ht="23" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-    </row>
-    <row r="16" spans="1:14" ht="23" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-    </row>
-    <row r="17" spans="1:8" ht="23" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="1:8" ht="23" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-    </row>
-    <row r="19" spans="1:8" ht="23" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="1:8" ht="23" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="1:8" ht="23" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="16" spans="1:14" ht="20" customHeight="1">
+      <c r="A16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" ht="20" customHeight="1">
+      <c r="A17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8" ht="19" customHeight="1">
+      <c r="A18" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:8" ht="20" customHeight="1">
+      <c r="A19" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:8" ht="17" customHeight="1">
+      <c r="A20" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="1:8" ht="20" customHeight="1">
+      <c r="A21" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="1:8" ht="20" customHeight="1">
+      <c r="A22" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
     </row>
     <row r="23" spans="1:8" ht="20" customHeight="1">
-      <c r="A23" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" ht="20" customHeight="1">
-      <c r="A24" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="A23" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="19" customHeight="1">
-      <c r="A25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:8" ht="20" customHeight="1">
-      <c r="A26" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="1:8" ht="17" customHeight="1">
-      <c r="A27" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="1:8" ht="20" customHeight="1">
-      <c r="A28" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="1:8" ht="20" customHeight="1">
-      <c r="A29" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" spans="1:8" ht="20" customHeight="1">
-      <c r="A30" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19" customHeight="1">
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="5:8" ht="46" customHeight="1">
-      <c r="E33" s="8" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:8" ht="46" customHeight="1">
+      <c r="E26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
+  <mergeCells count="30">
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="C7:F8"/>
+    <mergeCell ref="G7:H8"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="C7:F8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
   </mergeCells>
   <phoneticPr fontId="12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>